<commit_message>
Advanced Excel Formulas & Functions
</commit_message>
<xml_diff>
--- a/DatabaseAdministration/Excel/MicrosoftExcelAdvancedExcelFormulasAndFunctions/ExcelHomeworkExercises.xlsx
+++ b/DatabaseAdministration/Excel/MicrosoftExcelAdvancedExcelFormulasAndFunctions/ExcelHomeworkExercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Bhoola\Desktop\Pranav_Bhoola\DatabaseAdministration\Excel\MicrosoftExcelAdvancedExcelFormulasAndFunctions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643A2D61-62A1-4296-891C-FA247F7AD271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B506C210-55FF-43DF-B8D9-591D13F418E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="709" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="709" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulas 101" sheetId="19" r:id="rId1"/>
@@ -46,6 +46,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7702,7 +7724,7 @@
   </sheetPr>
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8984,7 +9006,9 @@
   </sheetPr>
   <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9028,7 +9052,10 @@
       <c r="D2" s="6">
         <v>177884</v>
       </c>
-      <c r="E2" s="45"/>
+      <c r="E2" s="45" t="str" cm="1">
+        <f t="array" ref="E2:E205">VLOOKUP(A2:A205,'State Abbreviations'!A2:B52,2)</f>
+        <v>AL</v>
+      </c>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9044,7 +9071,9 @@
       <c r="D3" s="6">
         <v>12538.64</v>
       </c>
-      <c r="E3" s="45"/>
+      <c r="E3" s="45" t="str">
+        <v>AK</v>
+      </c>
       <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9060,7 +9089,9 @@
       <c r="D4" s="6">
         <v>102612.64</v>
       </c>
-      <c r="E4" s="45"/>
+      <c r="E4" s="45" t="str">
+        <v>AZ</v>
+      </c>
       <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9076,7 +9107,9 @@
       <c r="D5" s="6">
         <v>53468</v>
       </c>
-      <c r="E5" s="45"/>
+      <c r="E5" s="45" t="str">
+        <v>AR</v>
+      </c>
       <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9092,7 +9125,9 @@
       <c r="D6" s="6">
         <v>1016149.44</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="45" t="str">
+        <v>CA</v>
+      </c>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9108,7 +9143,9 @@
       <c r="D7" s="6">
         <v>172050.44</v>
       </c>
-      <c r="E7" s="45"/>
+      <c r="E7" s="45" t="str">
+        <v>CO</v>
+      </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9124,7 +9161,9 @@
       <c r="D8" s="6">
         <v>102166.95</v>
       </c>
-      <c r="E8" s="45"/>
+      <c r="E8" s="45" t="str">
+        <v>CT</v>
+      </c>
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9140,7 +9179,9 @@
       <c r="D9" s="6">
         <v>23508</v>
       </c>
-      <c r="E9" s="45"/>
+      <c r="E9" s="45" t="str">
+        <v>DC</v>
+      </c>
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9156,7 +9197,9 @@
       <c r="D10" s="6">
         <v>17161.77</v>
       </c>
-      <c r="E10" s="45"/>
+      <c r="E10" s="45" t="str">
+        <v>DE</v>
+      </c>
       <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9172,7 +9215,9 @@
       <c r="D11" s="6">
         <v>319647.56</v>
       </c>
-      <c r="E11" s="45"/>
+      <c r="E11" s="45" t="str">
+        <v>FL</v>
+      </c>
       <c r="F11" s="42"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9188,7 +9233,9 @@
       <c r="D12" s="6">
         <v>245593.59</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="45" t="str">
+        <v>GA</v>
+      </c>
       <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9204,7 +9251,9 @@
       <c r="D13" s="6">
         <v>48461.48</v>
       </c>
-      <c r="E13" s="45"/>
+      <c r="E13" s="45" t="str">
+        <v>HI</v>
+      </c>
       <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9220,7 +9269,9 @@
       <c r="D14" s="6">
         <v>38818.589999999997</v>
       </c>
-      <c r="E14" s="45"/>
+      <c r="E14" s="45" t="str">
+        <v>ID</v>
+      </c>
       <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9236,7 +9287,9 @@
       <c r="D15" s="6">
         <v>496771.72000000003</v>
       </c>
-      <c r="E15" s="45"/>
+      <c r="E15" s="45" t="str">
+        <v>IL</v>
+      </c>
       <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9252,7 +9305,9 @@
       <c r="D16" s="6">
         <v>243219.4</v>
       </c>
-      <c r="E16" s="45"/>
+      <c r="E16" s="45" t="str">
+        <v>IN</v>
+      </c>
       <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9268,7 +9323,9 @@
       <c r="D17" s="6">
         <v>58526.48</v>
       </c>
-      <c r="E17" s="45"/>
+      <c r="E17" s="45" t="str">
+        <v>IA</v>
+      </c>
       <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9284,7 +9341,9 @@
       <c r="D18" s="6">
         <v>107536.72</v>
       </c>
-      <c r="E18" s="45"/>
+      <c r="E18" s="45" t="str">
+        <v>KS</v>
+      </c>
       <c r="F18" s="42"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9300,7 +9359,9 @@
       <c r="D19" s="6">
         <v>161670.76</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="45" t="str">
+        <v>KY</v>
+      </c>
       <c r="F19" s="42"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -9316,7 +9377,9 @@
       <c r="D20" s="6">
         <v>89379.520000000004</v>
       </c>
-      <c r="E20" s="45"/>
+      <c r="E20" s="45" t="str">
+        <v>LA</v>
+      </c>
       <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -9332,7 +9395,9 @@
       <c r="D21" s="6">
         <v>38247.689999999995</v>
       </c>
-      <c r="E21" s="45"/>
+      <c r="E21" s="45" t="str">
+        <v>ME</v>
+      </c>
       <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -9348,7 +9413,9 @@
       <c r="D22" s="6">
         <v>158894.57999999999</v>
       </c>
-      <c r="E22" s="45"/>
+      <c r="E22" s="45" t="str">
+        <v>MD</v>
+      </c>
       <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -9364,7 +9431,9 @@
       <c r="D23" s="6">
         <v>253963.88</v>
       </c>
-      <c r="E23" s="45"/>
+      <c r="E23" s="45" t="str">
+        <v>MA</v>
+      </c>
       <c r="F23" s="42"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -9380,7 +9449,9 @@
       <c r="D24" s="6">
         <v>198768.88</v>
       </c>
-      <c r="E24" s="45"/>
+      <c r="E24" s="45" t="str">
+        <v>MI</v>
+      </c>
       <c r="F24" s="42"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -9396,7 +9467,9 @@
       <c r="D25" s="6">
         <v>196779.16</v>
       </c>
-      <c r="E25" s="45"/>
+      <c r="E25" s="45" t="str">
+        <v>MN</v>
+      </c>
       <c r="F25" s="42"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -9412,7 +9485,9 @@
       <c r="D26" s="6">
         <v>85339.739999999991</v>
       </c>
-      <c r="E26" s="45"/>
+      <c r="E26" s="45" t="str">
+        <v>MS</v>
+      </c>
       <c r="F26" s="42"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -9428,7 +9503,9 @@
       <c r="D27" s="6">
         <v>111904.22</v>
       </c>
-      <c r="E27" s="45"/>
+      <c r="E27" s="45" t="str">
+        <v>MO</v>
+      </c>
       <c r="F27" s="42"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -9444,7 +9521,9 @@
       <c r="D28" s="6">
         <v>36087.800000000003</v>
       </c>
-      <c r="E28" s="45"/>
+      <c r="E28" s="45" t="str">
+        <v>MT</v>
+      </c>
       <c r="F28" s="42"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -9460,7 +9539,9 @@
       <c r="D29" s="6">
         <v>51337.89</v>
       </c>
-      <c r="E29" s="45"/>
+      <c r="E29" s="45" t="str">
+        <v>NE</v>
+      </c>
       <c r="F29" s="42"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -9476,7 +9557,9 @@
       <c r="D30" s="6">
         <v>79930.28</v>
       </c>
-      <c r="E30" s="45"/>
+      <c r="E30" s="45" t="str">
+        <v>NV</v>
+      </c>
       <c r="F30" s="42"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -9492,7 +9575,9 @@
       <c r="D31" s="6">
         <v>37073.58</v>
       </c>
-      <c r="E31" s="45"/>
+      <c r="E31" s="45" t="str">
+        <v>NH</v>
+      </c>
       <c r="F31" s="42"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -9508,7 +9593,9 @@
       <c r="D32" s="6">
         <v>336574</v>
       </c>
-      <c r="E32" s="45"/>
+      <c r="E32" s="45" t="str">
+        <v>NJ</v>
+      </c>
       <c r="F32" s="42"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -9524,7 +9611,9 @@
       <c r="D33" s="6">
         <v>54571.38</v>
       </c>
-      <c r="E33" s="45"/>
+      <c r="E33" s="45" t="str">
+        <v>NM</v>
+      </c>
       <c r="F33" s="42"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -9540,7 +9629,9 @@
       <c r="D34" s="6">
         <v>759058.28</v>
       </c>
-      <c r="E34" s="45"/>
+      <c r="E34" s="45" t="str">
+        <v>NY</v>
+      </c>
       <c r="F34" s="42"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -9556,7 +9647,9 @@
       <c r="D35" s="6">
         <v>241479.38999999998</v>
       </c>
-      <c r="E35" s="45"/>
+      <c r="E35" s="45" t="str">
+        <v>NC</v>
+      </c>
       <c r="F35" s="42"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -9572,7 +9665,9 @@
       <c r="D36" s="6">
         <v>25688</v>
       </c>
-      <c r="E36" s="45"/>
+      <c r="E36" s="45" t="str">
+        <v>ND</v>
+      </c>
       <c r="F36" s="42"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -9588,7 +9683,9 @@
       <c r="D37" s="6">
         <v>227062.80000000002</v>
       </c>
-      <c r="E37" s="45"/>
+      <c r="E37" s="45" t="str">
+        <v>OH</v>
+      </c>
       <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -9604,7 +9701,9 @@
       <c r="D38" s="6">
         <v>69013.08</v>
       </c>
-      <c r="E38" s="45"/>
+      <c r="E38" s="45" t="str">
+        <v>OK</v>
+      </c>
       <c r="F38" s="42"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -9620,7 +9719,9 @@
       <c r="D39" s="6">
         <v>68427.98</v>
       </c>
-      <c r="E39" s="45"/>
+      <c r="E39" s="45" t="str">
+        <v>OR</v>
+      </c>
       <c r="F39" s="42"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -9636,7 +9737,9 @@
       <c r="D40" s="6">
         <v>245621.08000000002</v>
       </c>
-      <c r="E40" s="45"/>
+      <c r="E40" s="45" t="str">
+        <v>PA</v>
+      </c>
       <c r="F40" s="42"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -9652,7 +9755,9 @@
       <c r="D41" s="6">
         <v>41932.76</v>
       </c>
-      <c r="E41" s="45"/>
+      <c r="E41" s="45" t="str">
+        <v>RI</v>
+      </c>
       <c r="F41" s="42"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -9668,7 +9773,9 @@
       <c r="D42" s="6">
         <v>160480.48000000001</v>
       </c>
-      <c r="E42" s="45"/>
+      <c r="E42" s="45" t="str">
+        <v>SC</v>
+      </c>
       <c r="F42" s="42"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -9684,7 +9791,9 @@
       <c r="D43" s="6">
         <v>30193.760000000002</v>
       </c>
-      <c r="E43" s="45"/>
+      <c r="E43" s="45" t="str">
+        <v>SD</v>
+      </c>
       <c r="F43" s="42"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -9700,7 +9809,9 @@
       <c r="D44" s="6">
         <v>170678.49</v>
       </c>
-      <c r="E44" s="45"/>
+      <c r="E44" s="45" t="str">
+        <v>TN</v>
+      </c>
       <c r="F44" s="42"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -9716,7 +9827,9 @@
       <c r="D45" s="6">
         <v>417036.4</v>
       </c>
-      <c r="E45" s="45"/>
+      <c r="E45" s="45" t="str">
+        <v>TX</v>
+      </c>
       <c r="F45" s="42"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -9732,7 +9845,9 @@
       <c r="D46" s="6">
         <v>66995.069999999992</v>
       </c>
-      <c r="E46" s="45"/>
+      <c r="E46" s="45" t="str">
+        <v>UT</v>
+      </c>
       <c r="F46" s="42"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -9748,7 +9863,9 @@
       <c r="D47" s="6">
         <v>18264.809999999998</v>
       </c>
-      <c r="E47" s="45"/>
+      <c r="E47" s="45" t="str">
+        <v>VT</v>
+      </c>
       <c r="F47" s="42"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -9764,7 +9881,9 @@
       <c r="D48" s="6">
         <v>212355.44999999998</v>
       </c>
-      <c r="E48" s="45"/>
+      <c r="E48" s="45" t="str">
+        <v>VA</v>
+      </c>
       <c r="F48" s="42"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -9780,7 +9899,9 @@
       <c r="D49" s="6">
         <v>176823.63</v>
       </c>
-      <c r="E49" s="45"/>
+      <c r="E49" s="45" t="str">
+        <v>WA</v>
+      </c>
       <c r="F49" s="42"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -9796,7 +9917,9 @@
       <c r="D50" s="6">
         <v>72333.759999999995</v>
       </c>
-      <c r="E50" s="45"/>
+      <c r="E50" s="45" t="str">
+        <v>WV</v>
+      </c>
       <c r="F50" s="42"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -9812,7 +9935,9 @@
       <c r="D51" s="6">
         <v>214547</v>
       </c>
-      <c r="E51" s="45"/>
+      <c r="E51" s="45" t="str">
+        <v>WI</v>
+      </c>
       <c r="F51" s="42"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -9828,7 +9953,9 @@
       <c r="D52" s="6">
         <v>19751.28</v>
       </c>
-      <c r="E52" s="45"/>
+      <c r="E52" s="45" t="str">
+        <v>WY</v>
+      </c>
       <c r="F52" s="42"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -9844,7 +9971,9 @@
       <c r="D53" s="6">
         <v>135905.46</v>
       </c>
-      <c r="E53" s="45"/>
+      <c r="E53" s="45" t="str">
+        <v>AL</v>
+      </c>
       <c r="F53" s="42"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -9860,7 +9989,9 @@
       <c r="D54" s="6">
         <v>19663.05</v>
       </c>
-      <c r="E54" s="45"/>
+      <c r="E54" s="45" t="str">
+        <v>AK</v>
+      </c>
       <c r="F54" s="42"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -9876,7 +10007,9 @@
       <c r="D55" s="6">
         <v>114876.68000000001</v>
       </c>
-      <c r="E55" s="45"/>
+      <c r="E55" s="45" t="str">
+        <v>AZ</v>
+      </c>
       <c r="F55" s="42"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -9892,7 +10025,9 @@
       <c r="D56" s="6">
         <v>110105.16</v>
       </c>
-      <c r="E56" s="45"/>
+      <c r="E56" s="45" t="str">
+        <v>AR</v>
+      </c>
       <c r="F56" s="42"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -9908,7 +10043,9 @@
       <c r="D57" s="6">
         <v>1076813.97</v>
       </c>
-      <c r="E57" s="45"/>
+      <c r="E57" s="45" t="str">
+        <v>CA</v>
+      </c>
       <c r="F57" s="42"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -9924,7 +10061,9 @@
       <c r="D58" s="6">
         <v>138042.09</v>
       </c>
-      <c r="E58" s="45"/>
+      <c r="E58" s="45" t="str">
+        <v>CO</v>
+      </c>
       <c r="F58" s="42"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -9940,7 +10079,9 @@
       <c r="D59" s="6">
         <v>140144.16</v>
       </c>
-      <c r="E59" s="45"/>
+      <c r="E59" s="45" t="str">
+        <v>CT</v>
+      </c>
       <c r="F59" s="42"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -9956,7 +10097,9 @@
       <c r="D60" s="6">
         <v>33214.559999999998</v>
       </c>
-      <c r="E60" s="45"/>
+      <c r="E60" s="45" t="str">
+        <v>DC</v>
+      </c>
       <c r="F60" s="42"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -9972,7 +10115,9 @@
       <c r="D61" s="6">
         <v>16605.689999999999</v>
       </c>
-      <c r="E61" s="45"/>
+      <c r="E61" s="45" t="str">
+        <v>DE</v>
+      </c>
       <c r="F61" s="42"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -9988,7 +10133,9 @@
       <c r="D62" s="6">
         <v>695886.44000000006</v>
       </c>
-      <c r="E62" s="45"/>
+      <c r="E62" s="45" t="str">
+        <v>FL</v>
+      </c>
       <c r="F62" s="42"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -10004,7 +10151,9 @@
       <c r="D63" s="6">
         <v>176587.66</v>
       </c>
-      <c r="E63" s="45"/>
+      <c r="E63" s="45" t="str">
+        <v>GA</v>
+      </c>
       <c r="F63" s="42"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -10020,7 +10169,9 @@
       <c r="D64" s="6">
         <v>50513.599999999999</v>
       </c>
-      <c r="E64" s="45"/>
+      <c r="E64" s="45" t="str">
+        <v>HI</v>
+      </c>
       <c r="F64" s="42"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -10036,7 +10187,9 @@
       <c r="D65" s="6">
         <v>55730.48</v>
       </c>
-      <c r="E65" s="45"/>
+      <c r="E65" s="45" t="str">
+        <v>ID</v>
+      </c>
       <c r="F65" s="42"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -10052,7 +10205,9 @@
       <c r="D66" s="6">
         <v>381409.01999999996</v>
       </c>
-      <c r="E66" s="45"/>
+      <c r="E66" s="45" t="str">
+        <v>IL</v>
+      </c>
       <c r="F66" s="42"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -10068,7 +10223,9 @@
       <c r="D67" s="6">
         <v>187127.07</v>
       </c>
-      <c r="E67" s="45"/>
+      <c r="E67" s="45" t="str">
+        <v>IN</v>
+      </c>
       <c r="F67" s="42"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -10084,7 +10241,9 @@
       <c r="D68" s="6">
         <v>59089.020000000004</v>
       </c>
-      <c r="E68" s="45"/>
+      <c r="E68" s="45" t="str">
+        <v>IA</v>
+      </c>
       <c r="F68" s="42"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -10100,7 +10259,9 @@
       <c r="D69" s="6">
         <v>109420.08</v>
       </c>
-      <c r="E69" s="45"/>
+      <c r="E69" s="45" t="str">
+        <v>KS</v>
+      </c>
       <c r="F69" s="42"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -10116,7 +10277,9 @@
       <c r="D70" s="6">
         <v>124377.65999999999</v>
       </c>
-      <c r="E70" s="45"/>
+      <c r="E70" s="45" t="str">
+        <v>KY</v>
+      </c>
       <c r="F70" s="42"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -10132,7 +10295,9 @@
       <c r="D71" s="6">
         <v>180630.80000000002</v>
       </c>
-      <c r="E71" s="45"/>
+      <c r="E71" s="45" t="str">
+        <v>LA</v>
+      </c>
       <c r="F71" s="42"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -10148,7 +10313,9 @@
       <c r="D72" s="6">
         <v>52690.12</v>
       </c>
-      <c r="E72" s="45"/>
+      <c r="E72" s="45" t="str">
+        <v>ME</v>
+      </c>
       <c r="F72" s="42"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -10164,7 +10331,9 @@
       <c r="D73" s="6">
         <v>111161.16</v>
       </c>
-      <c r="E73" s="45"/>
+      <c r="E73" s="45" t="str">
+        <v>MD</v>
+      </c>
       <c r="F73" s="42"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -10180,7 +10349,9 @@
       <c r="D74" s="6">
         <v>192495.15</v>
       </c>
-      <c r="E74" s="45"/>
+      <c r="E74" s="45" t="str">
+        <v>MA</v>
+      </c>
       <c r="F74" s="42"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -10196,7 +10367,9 @@
       <c r="D75" s="6">
         <v>202252.4</v>
       </c>
-      <c r="E75" s="45"/>
+      <c r="E75" s="45" t="str">
+        <v>MI</v>
+      </c>
       <c r="F75" s="42"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -10212,7 +10385,9 @@
       <c r="D76" s="6">
         <v>102019.16</v>
       </c>
-      <c r="E76" s="45"/>
+      <c r="E76" s="45" t="str">
+        <v>MN</v>
+      </c>
       <c r="F76" s="42"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -10228,7 +10403,9 @@
       <c r="D77" s="6">
         <v>58059.32</v>
       </c>
-      <c r="E77" s="45"/>
+      <c r="E77" s="45" t="str">
+        <v>MS</v>
+      </c>
       <c r="F77" s="42"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -10244,7 +10421,9 @@
       <c r="D78" s="6">
         <v>115092.36</v>
       </c>
-      <c r="E78" s="45"/>
+      <c r="E78" s="45" t="str">
+        <v>MO</v>
+      </c>
       <c r="F78" s="42"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -10260,7 +10439,9 @@
       <c r="D79" s="6">
         <v>27805.95</v>
       </c>
-      <c r="E79" s="45"/>
+      <c r="E79" s="45" t="str">
+        <v>MT</v>
+      </c>
       <c r="F79" s="42"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -10276,7 +10457,9 @@
       <c r="D80" s="6">
         <v>69888.56</v>
       </c>
-      <c r="E80" s="45"/>
+      <c r="E80" s="45" t="str">
+        <v>NE</v>
+      </c>
       <c r="F80" s="42"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -10292,7 +10475,9 @@
       <c r="D81" s="6">
         <v>93390.84</v>
       </c>
-      <c r="E81" s="45"/>
+      <c r="E81" s="45" t="str">
+        <v>NV</v>
+      </c>
       <c r="F81" s="42"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -10308,7 +10493,9 @@
       <c r="D82" s="6">
         <v>51980</v>
       </c>
-      <c r="E82" s="45"/>
+      <c r="E82" s="45" t="str">
+        <v>NH</v>
+      </c>
       <c r="F82" s="42"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -10324,7 +10511,9 @@
       <c r="D83" s="6">
         <v>260966.37</v>
       </c>
-      <c r="E83" s="45"/>
+      <c r="E83" s="45" t="str">
+        <v>NJ</v>
+      </c>
       <c r="F83" s="42"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -10340,7 +10529,9 @@
       <c r="D84" s="6">
         <v>76131.56</v>
       </c>
-      <c r="E84" s="45"/>
+      <c r="E84" s="45" t="str">
+        <v>NM</v>
+      </c>
       <c r="F84" s="42"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -10356,7 +10547,9 @@
       <c r="D85" s="6">
         <v>576812.64</v>
       </c>
-      <c r="E85" s="45"/>
+      <c r="E85" s="45" t="str">
+        <v>NY</v>
+      </c>
       <c r="F85" s="42"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -10372,7 +10565,9 @@
       <c r="D86" s="6">
         <v>341648.84</v>
       </c>
-      <c r="E86" s="45"/>
+      <c r="E86" s="45" t="str">
+        <v>NC</v>
+      </c>
       <c r="F86" s="42"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -10388,7 +10583,9 @@
       <c r="D87" s="6">
         <v>19030.98</v>
       </c>
-      <c r="E87" s="45"/>
+      <c r="E87" s="45" t="str">
+        <v>ND</v>
+      </c>
       <c r="F87" s="42"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -10404,7 +10601,9 @@
       <c r="D88" s="6">
         <v>343770.33</v>
       </c>
-      <c r="E88" s="45"/>
+      <c r="E88" s="45" t="str">
+        <v>OH</v>
+      </c>
       <c r="F88" s="42"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -10420,7 +10619,9 @@
       <c r="D89" s="6">
         <v>140942.12</v>
       </c>
-      <c r="E89" s="45"/>
+      <c r="E89" s="45" t="str">
+        <v>OK</v>
+      </c>
       <c r="F89" s="42"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -10436,7 +10637,9 @@
       <c r="D90" s="6">
         <v>143783.44</v>
       </c>
-      <c r="E90" s="45"/>
+      <c r="E90" s="45" t="str">
+        <v>OR</v>
+      </c>
       <c r="F90" s="42"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -10452,7 +10655,9 @@
       <c r="D91" s="6">
         <v>496251.68</v>
       </c>
-      <c r="E91" s="45"/>
+      <c r="E91" s="45" t="str">
+        <v>PA</v>
+      </c>
       <c r="F91" s="42"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -10468,7 +10673,9 @@
       <c r="D92" s="6">
         <v>43225.279999999999</v>
       </c>
-      <c r="E92" s="45"/>
+      <c r="E92" s="45" t="str">
+        <v>RI</v>
+      </c>
       <c r="F92" s="42"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -10484,7 +10691,9 @@
       <c r="D93" s="6">
         <v>83961.36</v>
       </c>
-      <c r="E93" s="45"/>
+      <c r="E93" s="45" t="str">
+        <v>SC</v>
+      </c>
       <c r="F93" s="42"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -10500,7 +10709,9 @@
       <c r="D94" s="6">
         <v>23126.489999999998</v>
       </c>
-      <c r="E94" s="45"/>
+      <c r="E94" s="45" t="str">
+        <v>SD</v>
+      </c>
       <c r="F94" s="42"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -10516,7 +10727,9 @@
       <c r="D95" s="6">
         <v>118019.24</v>
       </c>
-      <c r="E95" s="45"/>
+      <c r="E95" s="45" t="str">
+        <v>TN</v>
+      </c>
       <c r="F95" s="42"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -10532,7 +10745,9 @@
       <c r="D96" s="6">
         <v>950569.24</v>
       </c>
-      <c r="E96" s="45"/>
+      <c r="E96" s="45" t="str">
+        <v>TX</v>
+      </c>
       <c r="F96" s="42"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -10548,7 +10763,9 @@
       <c r="D97" s="6">
         <v>47780.78</v>
       </c>
-      <c r="E97" s="45"/>
+      <c r="E97" s="45" t="str">
+        <v>UT</v>
+      </c>
       <c r="F97" s="42"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -10564,7 +10781,9 @@
       <c r="D98" s="6">
         <v>12427.880000000001</v>
       </c>
-      <c r="E98" s="45"/>
+      <c r="E98" s="45" t="str">
+        <v>VT</v>
+      </c>
       <c r="F98" s="42"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -10580,7 +10799,9 @@
       <c r="D99" s="6">
         <v>298393.08</v>
       </c>
-      <c r="E99" s="45"/>
+      <c r="E99" s="45" t="str">
+        <v>VA</v>
+      </c>
       <c r="F99" s="42"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -10596,7 +10817,9 @@
       <c r="D100" s="6">
         <v>124075.76000000001</v>
       </c>
-      <c r="E100" s="45"/>
+      <c r="E100" s="45" t="str">
+        <v>WA</v>
+      </c>
       <c r="F100" s="42"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -10612,7 +10835,9 @@
       <c r="D101" s="6">
         <v>36307.08</v>
       </c>
-      <c r="E101" s="45"/>
+      <c r="E101" s="45" t="str">
+        <v>WV</v>
+      </c>
       <c r="F101" s="42"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -10628,7 +10853,9 @@
       <c r="D102" s="6">
         <v>220361.04</v>
       </c>
-      <c r="E102" s="45"/>
+      <c r="E102" s="45" t="str">
+        <v>WI</v>
+      </c>
       <c r="F102" s="42"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -10644,7 +10871,9 @@
       <c r="D103" s="6">
         <v>15195.869999999999</v>
       </c>
-      <c r="E103" s="45"/>
+      <c r="E103" s="45" t="str">
+        <v>WY</v>
+      </c>
       <c r="F103" s="42"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -10660,7 +10889,9 @@
       <c r="D104" s="6">
         <v>143392.04999999999</v>
       </c>
-      <c r="E104" s="45"/>
+      <c r="E104" s="45" t="str">
+        <v>AL</v>
+      </c>
       <c r="F104" s="42"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -10676,7 +10907,9 @@
       <c r="D105" s="6">
         <v>14204.62</v>
       </c>
-      <c r="E105" s="45"/>
+      <c r="E105" s="45" t="str">
+        <v>AK</v>
+      </c>
       <c r="F105" s="42"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -10692,7 +10925,9 @@
       <c r="D106" s="6">
         <v>126580.26000000001</v>
       </c>
-      <c r="E106" s="45"/>
+      <c r="E106" s="45" t="str">
+        <v>AZ</v>
+      </c>
       <c r="F106" s="42"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -10708,7 +10943,9 @@
       <c r="D107" s="6">
         <v>58318.42</v>
       </c>
-      <c r="E107" s="45"/>
+      <c r="E107" s="45" t="str">
+        <v>AR</v>
+      </c>
       <c r="F107" s="42"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -10724,7 +10961,9 @@
       <c r="D108" s="6">
         <v>745079.12</v>
       </c>
-      <c r="E108" s="45"/>
+      <c r="E108" s="45" t="str">
+        <v>CA</v>
+      </c>
       <c r="F108" s="42"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -10740,7 +10979,9 @@
       <c r="D109" s="6">
         <v>201167.84</v>
       </c>
-      <c r="E109" s="45"/>
+      <c r="E109" s="45" t="str">
+        <v>CO</v>
+      </c>
       <c r="F109" s="42"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -10756,7 +10997,9 @@
       <c r="D110" s="6">
         <v>142963.88</v>
       </c>
-      <c r="E110" s="45"/>
+      <c r="E110" s="45" t="str">
+        <v>CT</v>
+      </c>
       <c r="F110" s="42"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -10772,7 +11015,9 @@
       <c r="D111" s="6">
         <v>26938.02</v>
       </c>
-      <c r="E111" s="45"/>
+      <c r="E111" s="45" t="str">
+        <v>DC</v>
+      </c>
       <c r="F111" s="42"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -10788,7 +11033,9 @@
       <c r="D112" s="6">
         <v>18051.689999999999</v>
       </c>
-      <c r="E112" s="45"/>
+      <c r="E112" s="45" t="str">
+        <v>DE</v>
+      </c>
       <c r="F112" s="42"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -10804,7 +11051,9 @@
       <c r="D113" s="6">
         <v>752052.44000000006</v>
       </c>
-      <c r="E113" s="45"/>
+      <c r="E113" s="45" t="str">
+        <v>FL</v>
+      </c>
       <c r="F113" s="42"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -10820,7 +11069,9 @@
       <c r="D114" s="6">
         <v>193753.06</v>
       </c>
-      <c r="E114" s="45"/>
+      <c r="E114" s="45" t="str">
+        <v>GA</v>
+      </c>
       <c r="F114" s="42"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -10836,7 +11087,9 @@
       <c r="D115" s="6">
         <v>54412.04</v>
       </c>
-      <c r="E115" s="45"/>
+      <c r="E115" s="45" t="str">
+        <v>HI</v>
+      </c>
       <c r="F115" s="42"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -10852,7 +11105,9 @@
       <c r="D116" s="6">
         <v>47027.46</v>
       </c>
-      <c r="E116" s="45"/>
+      <c r="E116" s="45" t="str">
+        <v>ID</v>
+      </c>
       <c r="F116" s="42"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -10868,7 +11123,9 @@
       <c r="D117" s="6">
         <v>256612.64</v>
       </c>
-      <c r="E117" s="45"/>
+      <c r="E117" s="45" t="str">
+        <v>IL</v>
+      </c>
       <c r="F117" s="42"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -10884,7 +11141,9 @@
       <c r="D118" s="6">
         <v>259352</v>
       </c>
-      <c r="E118" s="45"/>
+      <c r="E118" s="45" t="str">
+        <v>IN</v>
+      </c>
       <c r="F118" s="42"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -10900,7 +11159,9 @@
       <c r="D119" s="6">
         <v>60927</v>
       </c>
-      <c r="E119" s="45"/>
+      <c r="E119" s="45" t="str">
+        <v>IA</v>
+      </c>
       <c r="F119" s="42"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -10916,7 +11177,9 @@
       <c r="D120" s="6">
         <v>85593.54</v>
       </c>
-      <c r="E120" s="45"/>
+      <c r="E120" s="45" t="str">
+        <v>KS</v>
+      </c>
       <c r="F120" s="42"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -10932,7 +11195,9 @@
       <c r="D121" s="6">
         <v>130180.86</v>
       </c>
-      <c r="E121" s="45"/>
+      <c r="E121" s="45" t="str">
+        <v>KY</v>
+      </c>
       <c r="F121" s="42"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -10948,7 +11213,9 @@
       <c r="D122" s="6">
         <v>136001.16</v>
       </c>
-      <c r="E122" s="45"/>
+      <c r="E122" s="45" t="str">
+        <v>LA</v>
+      </c>
       <c r="F122" s="42"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -10964,7 +11231,9 @@
       <c r="D123" s="6">
         <v>26567.22</v>
       </c>
-      <c r="E123" s="45"/>
+      <c r="E123" s="45" t="str">
+        <v>ME</v>
+      </c>
       <c r="F123" s="42"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -10980,7 +11249,9 @@
       <c r="D124" s="6">
         <v>230942.08000000002</v>
       </c>
-      <c r="E124" s="45"/>
+      <c r="E124" s="45" t="str">
+        <v>MD</v>
+      </c>
       <c r="F124" s="42"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -10996,7 +11267,9 @@
       <c r="D125" s="6">
         <v>130952.58</v>
       </c>
-      <c r="E125" s="45"/>
+      <c r="E125" s="45" t="str">
+        <v>MA</v>
+      </c>
       <c r="F125" s="42"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -11012,7 +11285,9 @@
       <c r="D126" s="6">
         <v>197672.7</v>
       </c>
-      <c r="E126" s="45"/>
+      <c r="E126" s="45" t="str">
+        <v>MI</v>
+      </c>
       <c r="F126" s="42"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -11028,7 +11303,9 @@
       <c r="D127" s="6">
         <v>106078.5</v>
       </c>
-      <c r="E127" s="45"/>
+      <c r="E127" s="45" t="str">
+        <v>MN</v>
+      </c>
       <c r="F127" s="42"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -11044,7 +11321,9 @@
       <c r="D128" s="6">
         <v>89018.91</v>
       </c>
-      <c r="E128" s="45"/>
+      <c r="E128" s="45" t="str">
+        <v>MS</v>
+      </c>
       <c r="F128" s="42"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -11060,7 +11339,9 @@
       <c r="D129" s="6">
         <v>119778.54000000001</v>
       </c>
-      <c r="E129" s="45"/>
+      <c r="E129" s="45" t="str">
+        <v>MO</v>
+      </c>
       <c r="F129" s="42"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -11076,7 +11357,9 @@
       <c r="D130" s="6">
         <v>29682.449999999997</v>
       </c>
-      <c r="E130" s="45"/>
+      <c r="E130" s="45" t="str">
+        <v>MT</v>
+      </c>
       <c r="F130" s="42"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -11092,7 +11375,9 @@
       <c r="D131" s="6">
         <v>36526.82</v>
       </c>
-      <c r="E131" s="45"/>
+      <c r="E131" s="45" t="str">
+        <v>NE</v>
+      </c>
       <c r="F131" s="42"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -11108,7 +11393,9 @@
       <c r="D132" s="6">
         <v>81016.53</v>
       </c>
-      <c r="E132" s="45"/>
+      <c r="E132" s="45" t="str">
+        <v>NV</v>
+      </c>
       <c r="F132" s="42"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -11124,7 +11411,9 @@
       <c r="D133" s="6">
         <v>26329.440000000002</v>
       </c>
-      <c r="E133" s="45"/>
+      <c r="E133" s="45" t="str">
+        <v>NH</v>
+      </c>
       <c r="F133" s="42"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -11140,7 +11429,9 @@
       <c r="D134" s="6">
         <v>263756.82</v>
       </c>
-      <c r="E134" s="45"/>
+      <c r="E134" s="45" t="str">
+        <v>NJ</v>
+      </c>
       <c r="F134" s="42"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -11156,7 +11447,9 @@
       <c r="D135" s="6">
         <v>61775.399999999994</v>
       </c>
-      <c r="E135" s="45"/>
+      <c r="E135" s="45" t="str">
+        <v>NM</v>
+      </c>
       <c r="F135" s="42"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -11172,7 +11465,9 @@
       <c r="D136" s="6">
         <v>387562.08</v>
       </c>
-      <c r="E136" s="45"/>
+      <c r="E136" s="45" t="str">
+        <v>NY</v>
+      </c>
       <c r="F136" s="42"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -11188,7 +11483,9 @@
       <c r="D137" s="6">
         <v>190709.5</v>
       </c>
-      <c r="E137" s="45"/>
+      <c r="E137" s="45" t="str">
+        <v>NC</v>
+      </c>
       <c r="F137" s="42"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -11204,7 +11501,9 @@
       <c r="D138" s="6">
         <v>20177.73</v>
       </c>
-      <c r="E138" s="45"/>
+      <c r="E138" s="45" t="str">
+        <v>ND</v>
+      </c>
       <c r="F138" s="42"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -11220,7 +11519,9 @@
       <c r="D139" s="6">
         <v>346095.06</v>
       </c>
-      <c r="E139" s="45"/>
+      <c r="E139" s="45" t="str">
+        <v>OH</v>
+      </c>
       <c r="F139" s="42"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -11236,7 +11537,9 @@
       <c r="D140" s="6">
         <v>112540.62</v>
       </c>
-      <c r="E140" s="45"/>
+      <c r="E140" s="45" t="str">
+        <v>OK</v>
+      </c>
       <c r="F140" s="42"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -11252,7 +11555,9 @@
       <c r="D141" s="6">
         <v>114932.22</v>
       </c>
-      <c r="E141" s="45"/>
+      <c r="E141" s="45" t="str">
+        <v>OR</v>
+      </c>
       <c r="F141" s="42"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -11268,7 +11573,9 @@
       <c r="D142" s="6">
         <v>254047.58000000002</v>
       </c>
-      <c r="E142" s="45"/>
+      <c r="E142" s="45" t="str">
+        <v>PA</v>
+      </c>
       <c r="F142" s="42"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -11284,7 +11591,9 @@
       <c r="D143" s="6">
         <v>42102.68</v>
       </c>
-      <c r="E143" s="45"/>
+      <c r="E143" s="45" t="str">
+        <v>RI</v>
+      </c>
       <c r="F143" s="42"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -11300,7 +11609,9 @@
       <c r="D144" s="6">
         <v>138760.91999999998</v>
       </c>
-      <c r="E144" s="45"/>
+      <c r="E144" s="45" t="str">
+        <v>SC</v>
+      </c>
       <c r="F144" s="42"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -11316,7 +11627,9 @@
       <c r="D145" s="6">
         <v>24425.399999999998</v>
       </c>
-      <c r="E145" s="45"/>
+      <c r="E145" s="45" t="str">
+        <v>SD</v>
+      </c>
       <c r="F145" s="42"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -11332,7 +11645,9 @@
       <c r="D146" s="6">
         <v>253844.4</v>
       </c>
-      <c r="E146" s="45"/>
+      <c r="E146" s="45" t="str">
+        <v>TN</v>
+      </c>
       <c r="F146" s="42"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -11348,7 +11663,9 @@
       <c r="D147" s="6">
         <v>754366.83</v>
       </c>
-      <c r="E147" s="45"/>
+      <c r="E147" s="45" t="str">
+        <v>TX</v>
+      </c>
       <c r="F147" s="42"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -11364,7 +11681,9 @@
       <c r="D148" s="6">
         <v>55277.700000000004</v>
       </c>
-      <c r="E148" s="45"/>
+      <c r="E148" s="45" t="str">
+        <v>UT</v>
+      </c>
       <c r="F148" s="42"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -11380,7 +11699,9 @@
       <c r="D149" s="6">
         <v>12514.82</v>
       </c>
-      <c r="E149" s="45"/>
+      <c r="E149" s="45" t="str">
+        <v>VT</v>
+      </c>
       <c r="F149" s="42"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -11396,7 +11717,9 @@
       <c r="D150" s="6">
         <v>240030.72</v>
       </c>
-      <c r="E150" s="45"/>
+      <c r="E150" s="45" t="str">
+        <v>VA</v>
+      </c>
       <c r="F150" s="42"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -11412,7 +11735,9 @@
       <c r="D151" s="6">
         <v>268981.59999999998</v>
       </c>
-      <c r="E151" s="45"/>
+      <c r="E151" s="45" t="str">
+        <v>WA</v>
+      </c>
       <c r="F151" s="42"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -11428,7 +11753,9 @@
       <c r="D152" s="6">
         <v>37059.919999999998</v>
       </c>
-      <c r="E152" s="45"/>
+      <c r="E152" s="45" t="str">
+        <v>WV</v>
+      </c>
       <c r="F152" s="42"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -11444,7 +11771,9 @@
       <c r="D153" s="6">
         <v>113739.72</v>
       </c>
-      <c r="E153" s="45"/>
+      <c r="E153" s="45" t="str">
+        <v>WI</v>
+      </c>
       <c r="F153" s="42"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -11460,7 +11789,9 @@
       <c r="D154" s="6">
         <v>11272.52</v>
       </c>
-      <c r="E154" s="45"/>
+      <c r="E154" s="45" t="str">
+        <v>WY</v>
+      </c>
       <c r="F154" s="42"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -11476,7 +11807,9 @@
       <c r="D155" s="6">
         <v>96440.46</v>
       </c>
-      <c r="E155" s="45"/>
+      <c r="E155" s="45" t="str">
+        <v>AL</v>
+      </c>
       <c r="F155" s="42"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -11492,7 +11825,9 @@
       <c r="D156" s="6">
         <v>14628.98</v>
       </c>
-      <c r="E156" s="45"/>
+      <c r="E156" s="45" t="str">
+        <v>AK</v>
+      </c>
       <c r="F156" s="42"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -11508,7 +11843,9 @@
       <c r="D157" s="6">
         <v>262130.2</v>
       </c>
-      <c r="E157" s="45"/>
+      <c r="E157" s="45" t="str">
+        <v>AZ</v>
+      </c>
       <c r="F157" s="42"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -11524,7 +11861,9 @@
       <c r="D158" s="6">
         <v>88473.93</v>
       </c>
-      <c r="E158" s="45"/>
+      <c r="E158" s="45" t="str">
+        <v>AR</v>
+      </c>
       <c r="F158" s="42"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -11540,7 +11879,9 @@
       <c r="D159" s="6">
         <v>1141242.8999999999</v>
       </c>
-      <c r="E159" s="45"/>
+      <c r="E159" s="45" t="str">
+        <v>CA</v>
+      </c>
       <c r="F159" s="42"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -11556,7 +11897,9 @@
       <c r="D160" s="6">
         <v>155627.46</v>
       </c>
-      <c r="E160" s="45"/>
+      <c r="E160" s="45" t="str">
+        <v>CO</v>
+      </c>
       <c r="F160" s="42"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -11572,7 +11915,9 @@
       <c r="D161" s="6">
         <v>71806.94</v>
       </c>
-      <c r="E161" s="45"/>
+      <c r="E161" s="45" t="str">
+        <v>CT</v>
+      </c>
       <c r="F161" s="42"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -11588,7 +11933,9 @@
       <c r="D162" s="6">
         <v>18341.84</v>
       </c>
-      <c r="E162" s="45"/>
+      <c r="E162" s="45" t="str">
+        <v>DC</v>
+      </c>
       <c r="F162" s="42"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -11604,7 +11951,9 @@
       <c r="D163" s="6">
         <v>25292.920000000002</v>
       </c>
-      <c r="E163" s="45"/>
+      <c r="E163" s="45" t="str">
+        <v>DE</v>
+      </c>
       <c r="F163" s="42"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -11620,7 +11969,9 @@
       <c r="D164" s="6">
         <v>579527.03999999992</v>
       </c>
-      <c r="E164" s="45"/>
+      <c r="E164" s="45" t="str">
+        <v>FL</v>
+      </c>
       <c r="F164" s="42"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -11636,7 +11987,9 @@
       <c r="D165" s="6">
         <v>396797.8</v>
       </c>
-      <c r="E165" s="45"/>
+      <c r="E165" s="45" t="str">
+        <v>GA</v>
+      </c>
       <c r="F165" s="42"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -11652,7 +12005,9 @@
       <c r="D166" s="6">
         <v>55692.520000000004</v>
       </c>
-      <c r="E166" s="45"/>
+      <c r="E166" s="45" t="str">
+        <v>HI</v>
+      </c>
       <c r="F166" s="42"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -11668,7 +12023,9 @@
       <c r="D167" s="6">
         <v>31914.560000000001</v>
       </c>
-      <c r="E167" s="45"/>
+      <c r="E167" s="45" t="str">
+        <v>ID</v>
+      </c>
       <c r="F167" s="42"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -11684,7 +12041,9 @@
       <c r="D168" s="6">
         <v>386257.64999999997</v>
       </c>
-      <c r="E168" s="45"/>
+      <c r="E168" s="45" t="str">
+        <v>IL</v>
+      </c>
       <c r="F168" s="42"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -11700,7 +12059,9 @@
       <c r="D169" s="6">
         <v>261493.36000000002</v>
       </c>
-      <c r="E169" s="45"/>
+      <c r="E169" s="45" t="str">
+        <v>IN</v>
+      </c>
       <c r="F169" s="42"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -11716,7 +12077,9 @@
       <c r="D170" s="6">
         <v>122967.44</v>
       </c>
-      <c r="E170" s="45"/>
+      <c r="E170" s="45" t="str">
+        <v>IA</v>
+      </c>
       <c r="F170" s="42"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -11732,7 +12095,9 @@
       <c r="D171" s="6">
         <v>86577.15</v>
       </c>
-      <c r="E171" s="45"/>
+      <c r="E171" s="45" t="str">
+        <v>KS</v>
+      </c>
       <c r="F171" s="42"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -11748,7 +12113,9 @@
       <c r="D172" s="6">
         <v>175216.6</v>
       </c>
-      <c r="E172" s="45"/>
+      <c r="E172" s="45" t="str">
+        <v>KY</v>
+      </c>
       <c r="F172" s="42"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -11764,7 +12131,9 @@
       <c r="D173" s="6">
         <v>92037.86</v>
       </c>
-      <c r="E173" s="45"/>
+      <c r="E173" s="45" t="str">
+        <v>LA</v>
+      </c>
       <c r="F173" s="42"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -11780,7 +12149,9 @@
       <c r="D174" s="6">
         <v>39875.760000000002</v>
       </c>
-      <c r="E174" s="45"/>
+      <c r="E174" s="45" t="str">
+        <v>ME</v>
+      </c>
       <c r="F174" s="42"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
@@ -11796,7 +12167,9 @@
       <c r="D175" s="6">
         <v>235382.52000000002</v>
       </c>
-      <c r="E175" s="45"/>
+      <c r="E175" s="45" t="str">
+        <v>MD</v>
+      </c>
       <c r="F175" s="42"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
@@ -11812,7 +12185,9 @@
       <c r="D176" s="6">
         <v>265845.76000000001</v>
       </c>
-      <c r="E176" s="45"/>
+      <c r="E176" s="45" t="str">
+        <v>MA</v>
+      </c>
       <c r="F176" s="42"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
@@ -11828,7 +12203,9 @@
       <c r="D177" s="6">
         <v>296500.8</v>
       </c>
-      <c r="E177" s="45"/>
+      <c r="E177" s="45" t="str">
+        <v>MI</v>
+      </c>
       <c r="F177" s="42"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
@@ -11844,7 +12221,9 @@
       <c r="D178" s="6">
         <v>107582.78</v>
       </c>
-      <c r="E178" s="45"/>
+      <c r="E178" s="45" t="str">
+        <v>MN</v>
+      </c>
       <c r="F178" s="42"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -11860,7 +12239,9 @@
       <c r="D179" s="6">
         <v>119397.04000000001</v>
       </c>
-      <c r="E179" s="45"/>
+      <c r="E179" s="45" t="str">
+        <v>MS</v>
+      </c>
       <c r="F179" s="42"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
@@ -11876,7 +12257,9 @@
       <c r="D180" s="6">
         <v>120439.76000000001</v>
       </c>
-      <c r="E180" s="45"/>
+      <c r="E180" s="45" t="str">
+        <v>MO</v>
+      </c>
       <c r="F180" s="42"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -11892,7 +12275,9 @@
       <c r="D181" s="6">
         <v>40205.64</v>
       </c>
-      <c r="E181" s="45"/>
+      <c r="E181" s="45" t="str">
+        <v>MT</v>
+      </c>
       <c r="F181" s="42"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -11908,7 +12293,9 @@
       <c r="D182" s="6">
         <v>55665.75</v>
       </c>
-      <c r="E182" s="45"/>
+      <c r="E182" s="45" t="str">
+        <v>NE</v>
+      </c>
       <c r="F182" s="42"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
@@ -11924,7 +12311,9 @@
       <c r="D183" s="6">
         <v>110357.24</v>
       </c>
-      <c r="E183" s="45"/>
+      <c r="E183" s="45" t="str">
+        <v>NV</v>
+      </c>
       <c r="F183" s="42"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -11940,7 +12329,9 @@
       <c r="D184" s="6">
         <v>52828.72</v>
       </c>
-      <c r="E184" s="45"/>
+      <c r="E184" s="45" t="str">
+        <v>NH</v>
+      </c>
       <c r="F184" s="42"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -11956,7 +12347,9 @@
       <c r="D185" s="6">
         <v>177291.80000000002</v>
       </c>
-      <c r="E185" s="45"/>
+      <c r="E185" s="45" t="str">
+        <v>NJ</v>
+      </c>
       <c r="F185" s="42"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -11972,7 +12365,9 @@
       <c r="D186" s="6">
         <v>83421.52</v>
       </c>
-      <c r="E186" s="45"/>
+      <c r="E186" s="45" t="str">
+        <v>NM</v>
+      </c>
       <c r="F186" s="42"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -11988,7 +12383,9 @@
       <c r="D187" s="6">
         <v>587107.82999999996</v>
       </c>
-      <c r="E187" s="45"/>
+      <c r="E187" s="45" t="str">
+        <v>NY</v>
+      </c>
       <c r="F187" s="42"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -12004,7 +12401,9 @@
       <c r="D188" s="6">
         <v>195041.46</v>
       </c>
-      <c r="E188" s="45"/>
+      <c r="E188" s="45" t="str">
+        <v>NC</v>
+      </c>
       <c r="F188" s="42"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -12020,7 +12419,9 @@
       <c r="D189" s="6">
         <v>27985.119999999999</v>
       </c>
-      <c r="E189" s="45"/>
+      <c r="E189" s="45" t="str">
+        <v>ND</v>
+      </c>
       <c r="F189" s="42"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -12036,7 +12437,9 @@
       <c r="D190" s="6">
         <v>230884.5</v>
       </c>
-      <c r="E190" s="45"/>
+      <c r="E190" s="45" t="str">
+        <v>OH</v>
+      </c>
       <c r="F190" s="42"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -12052,7 +12455,9 @@
       <c r="D191" s="6">
         <v>152592.80000000002</v>
       </c>
-      <c r="E191" s="45"/>
+      <c r="E191" s="45" t="str">
+        <v>OK</v>
+      </c>
       <c r="F191" s="42"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -12068,7 +12473,9 @@
       <c r="D192" s="6">
         <v>77987.06</v>
       </c>
-      <c r="E192" s="45"/>
+      <c r="E192" s="45" t="str">
+        <v>OR</v>
+      </c>
       <c r="F192" s="42"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -12084,7 +12491,9 @@
       <c r="D193" s="6">
         <v>382906.07999999996</v>
       </c>
-      <c r="E193" s="45"/>
+      <c r="E193" s="45" t="str">
+        <v>PA</v>
+      </c>
       <c r="F193" s="42"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -12100,7 +12509,9 @@
       <c r="D194" s="6">
         <v>31508.76</v>
       </c>
-      <c r="E194" s="45"/>
+      <c r="E194" s="45" t="str">
+        <v>RI</v>
+      </c>
       <c r="F194" s="42"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -12116,7 +12527,9 @@
       <c r="D195" s="6">
         <v>141711.69</v>
       </c>
-      <c r="E195" s="45"/>
+      <c r="E195" s="45" t="str">
+        <v>SC</v>
+      </c>
       <c r="F195" s="42"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -12132,7 +12545,9 @@
       <c r="D196" s="6">
         <v>33334.160000000003</v>
       </c>
-      <c r="E196" s="45"/>
+      <c r="E196" s="45" t="str">
+        <v>SD</v>
+      </c>
       <c r="F196" s="42"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -12148,7 +12563,9 @@
       <c r="D197" s="6">
         <v>258249.72</v>
       </c>
-      <c r="E197" s="45"/>
+      <c r="E197" s="45" t="str">
+        <v>TN</v>
+      </c>
       <c r="F197" s="42"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -12164,7 +12581,9 @@
       <c r="D198" s="6">
         <v>1042368.12</v>
       </c>
-      <c r="E198" s="45"/>
+      <c r="E198" s="45" t="str">
+        <v>TX</v>
+      </c>
       <c r="F198" s="42"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -12180,7 +12599,9 @@
       <c r="D199" s="6">
         <v>114211.48</v>
       </c>
-      <c r="E199" s="45"/>
+      <c r="E199" s="45" t="str">
+        <v>UT</v>
+      </c>
       <c r="F199" s="42"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -12196,7 +12617,9 @@
       <c r="D200" s="6">
         <v>25040.440000000002</v>
       </c>
-      <c r="E200" s="45"/>
+      <c r="E200" s="45" t="str">
+        <v>VT</v>
+      </c>
       <c r="F200" s="42"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -12212,7 +12635,9 @@
       <c r="D201" s="6">
         <v>163717.34</v>
       </c>
-      <c r="E201" s="45"/>
+      <c r="E201" s="45" t="str">
+        <v>VA</v>
+      </c>
       <c r="F201" s="42"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -12228,7 +12653,9 @@
       <c r="D202" s="6">
         <v>137940.24</v>
       </c>
-      <c r="E202" s="45"/>
+      <c r="E202" s="45" t="str">
+        <v>WA</v>
+      </c>
       <c r="F202" s="42"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
@@ -12244,7 +12671,9 @@
       <c r="D203" s="6">
         <v>74216.52</v>
       </c>
-      <c r="E203" s="45"/>
+      <c r="E203" s="45" t="str">
+        <v>WV</v>
+      </c>
       <c r="F203" s="42"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
@@ -12260,7 +12689,9 @@
       <c r="D204" s="6">
         <v>114527.96</v>
       </c>
-      <c r="E204" s="45"/>
+      <c r="E204" s="45" t="str">
+        <v>WI</v>
+      </c>
       <c r="F204" s="42"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
@@ -12276,7 +12707,9 @@
       <c r="D205" s="6">
         <v>11528.24</v>
       </c>
-      <c r="E205" s="45"/>
+      <c r="E205" s="45" t="str">
+        <v>WY</v>
+      </c>
       <c r="F205" s="42"/>
     </row>
   </sheetData>

</xml_diff>